<commit_message>
Resolved Many Compiler Warnings In Controller Classes
</commit_message>
<xml_diff>
--- a/Sprints/CapstoneProjectProductBacklog.xlsx
+++ b/Sprints/CapstoneProjectProductBacklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdena1\source\repos\Capstone-Project\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16202AC0-AFCC-4A4E-9F29-51D2F5B7DA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E523851-B975-4F5A-97D2-B8FC887A8CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-870" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -237,7 +237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>